<commit_message>
update docs for header gen
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="379">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -585,7 +585,7 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RX_SADDR</t>
+    <t xml:space="preserve">RX_SADDR</t>
   </si>
   <si>
     <t xml:space="preserve">0x0</t>
@@ -600,7 +600,7 @@
     <t xml:space="preserve">RX SDIO uDMA transfer address of associated buffer</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RX_SIZE</t>
+    <t xml:space="preserve">RX_SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">0x4</t>
@@ -609,7 +609,7 @@
     <t xml:space="preserve">RX SDIO uDMA transfer size of buffer</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RX_CFG</t>
+    <t xml:space="preserve">RX_CFG</t>
   </si>
   <si>
     <t xml:space="preserve">0x8</t>
@@ -618,7 +618,7 @@
     <t xml:space="preserve">RX SDIO uDMA transfer configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RX_INITCFG</t>
+    <t xml:space="preserve">RX_INITCFG</t>
   </si>
   <si>
     <t xml:space="preserve">0xC</t>
@@ -627,7 +627,7 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_TX_SADDR</t>
+    <t xml:space="preserve">TX_SADDR</t>
   </si>
   <si>
     <t xml:space="preserve">0x10</t>
@@ -636,7 +636,7 @@
     <t xml:space="preserve">TX SDIO uDMA transfer address of associated buffer</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_TX_SIZE</t>
+    <t xml:space="preserve">TX_SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">0x14</t>
@@ -645,7 +645,7 @@
     <t xml:space="preserve">TX SDIO uDMA transfer size of buffer</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_TX_CFG</t>
+    <t xml:space="preserve">TX_CFG</t>
   </si>
   <si>
     <t xml:space="preserve">0x18</t>
@@ -654,13 +654,13 @@
     <t xml:space="preserve">TX SDIO uDMA transfer configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_TX_INITCFG</t>
+    <t xml:space="preserve">TX_INITCFG</t>
   </si>
   <si>
     <t xml:space="preserve">0x1C</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_CMD_OP</t>
+    <t xml:space="preserve">CMD_OP</t>
   </si>
   <si>
     <t xml:space="preserve">0x20</t>
@@ -675,7 +675,7 @@
     <t xml:space="preserve">SDIO command</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_CMD_ARG</t>
+    <t xml:space="preserve">CMD_ARG</t>
   </si>
   <si>
     <t xml:space="preserve">0x24</t>
@@ -684,7 +684,7 @@
     <t xml:space="preserve">SDIO argument</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_DATA_SETUP</t>
+    <t xml:space="preserve">DATA_SETUP</t>
   </si>
   <si>
     <t xml:space="preserve">0x28</t>
@@ -693,7 +693,7 @@
     <t xml:space="preserve">Data transfer setup</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_START</t>
+    <t xml:space="preserve">START</t>
   </si>
   <si>
     <t xml:space="preserve">0x2C</t>
@@ -702,7 +702,7 @@
     <t xml:space="preserve">Start</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RSP0</t>
+    <t xml:space="preserve">RSP0</t>
   </si>
   <si>
     <t xml:space="preserve">0x30</t>
@@ -711,7 +711,7 @@
     <t xml:space="preserve">Response byte0</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RSP1</t>
+    <t xml:space="preserve">RSP1</t>
   </si>
   <si>
     <t xml:space="preserve">0x34</t>
@@ -720,7 +720,7 @@
     <t xml:space="preserve">Response byte1</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RSP2</t>
+    <t xml:space="preserve">RSP2</t>
   </si>
   <si>
     <t xml:space="preserve">0x38</t>
@@ -729,7 +729,7 @@
     <t xml:space="preserve">Response byte2</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RSP3</t>
+    <t xml:space="preserve">RSP3</t>
   </si>
   <si>
     <t xml:space="preserve">0x3C</t>
@@ -738,7 +738,7 @@
     <t xml:space="preserve">Response byte3</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_CLK_DIV</t>
+    <t xml:space="preserve">CLK_DIV</t>
   </si>
   <si>
     <t xml:space="preserve">0x40</t>
@@ -747,16 +747,13 @@
     <t xml:space="preserve">Clock Divider</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_STATUS</t>
+    <t xml:space="preserve">STATUS</t>
   </si>
   <si>
     <t xml:space="preserve">0x44</t>
   </si>
   <si>
-    <t xml:space="preserve">STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_STOPCMD_OP</t>
+    <t xml:space="preserve">STOPCMD_OP</t>
   </si>
   <si>
     <t xml:space="preserve">0x48</t>
@@ -765,10 +762,10 @@
     <t xml:space="preserve">SDIO STOP command op</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_STOPCMD_ARG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x52</t>
+    <t xml:space="preserve">STOPCMD_ARG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4C</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO STOP command arg</t>
@@ -781,17 +778,11 @@
   </si>
   <si>
     <t xml:space="preserve">Bit Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX_SADDR</t>
   </si>
   <si>
     <t xml:space="preserve">Configure pointer to memory buffer:
 - Read: value of the pointer until transfer is over. Else returns 0
 - Write: set Address Pointer to memory buffer start address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX_SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">Buffer size in bytes. (1MBytes maximum)
@@ -844,12 +835,6 @@
     <t xml:space="preserve">Transfer pending in queue status flag:
 -1'b0: free
 -1'b1: pending</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX_SADDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX_SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">CMD_RSP_TYPE</t>
@@ -863,13 +848,7 @@
 -3’b100: 48 bits with BUSY check</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD_OP</t>
-  </si>
-  <si>
     <t xml:space="preserve">SDIO command opcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMD_ARG</t>
   </si>
   <si>
     <t xml:space="preserve">Argument to be sent with the command</t>
@@ -905,9 +884,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sets the block size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START</t>
   </si>
   <si>
     <t xml:space="preserve">Starts the SDIO transfer</t>
@@ -959,13 +935,13 @@
 -6'b00001: Response Time Out</t>
   </si>
   <si>
-    <t xml:space="preserve">STOPCMD_OP</t>
-  </si>
-  <si>
     <t xml:space="preserve">SDIO STOP command opcode</t>
   </si>
   <si>
     <t xml:space="preserve">STOPCMD_RSP_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_STOPCMD_OP</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO STOP command response type:
@@ -976,13 +952,13 @@
 -3’b100: 48 bits with BUSY check</t>
   </si>
   <si>
-    <t xml:space="preserve">STOPCMD_ARG</t>
+    <t xml:space="preserve">SDIO_STOPCMD_ARG</t>
   </si>
   <si>
     <t xml:space="preserve">Argument to be sent with the STOP command</t>
   </si>
   <si>
-    <t xml:space="preserve">CLK_DIV</t>
+    <t xml:space="preserve">SDIO_CLK_DIV</t>
   </si>
   <si>
     <t xml:space="preserve">Clock diviser</t>
@@ -1129,7 +1105,19 @@
     <t xml:space="preserve">0x1</t>
   </si>
   <si>
+    <t xml:space="preserve">0x37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x11</t>
+  </si>
+  <si>
     <t xml:space="preserve">0X1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x19</t>
   </si>
   <si>
     <t xml:space="preserve">UDMA_GC-&gt;CG</t>
@@ -2199,24 +2187,24 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>11</v>
@@ -2226,67 +2214,67 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="70" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,16 +2284,16 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,86 +2303,86 @@
     </row>
     <row r="18" customFormat="false" ht="158.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B18" s="60" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B19" s="60" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="176.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="160.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B23" s="60" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2432,10 +2420,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>11</v>
@@ -3664,10 +3652,10 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3717,7 +3705,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
         <v>169</v>
       </c>
@@ -3829,7 +3817,7 @@
       <c r="J5" s="59"/>
       <c r="K5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
         <v>183</v>
       </c>
@@ -4182,7 +4170,7 @@
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -4191,10 +4179,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="59" t="s">
         <v>226</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>227</v>
       </c>
       <c r="D20" s="36" t="n">
         <v>14</v>
@@ -4209,15 +4197,15 @@
         <v>170</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="59" t="s">
         <v>229</v>
-      </c>
-      <c r="C21" s="59" t="s">
-        <v>230</v>
       </c>
       <c r="D21" s="36" t="n">
         <v>32</v>
@@ -4232,7 +4220,7 @@
         <v>170</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4262,9 +4250,9 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4282,13 +4270,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="C1" s="45" t="s">
         <v>233</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>234</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -4306,9 +4294,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>235</v>
+        <v>169</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>169</v>
@@ -4329,12 +4317,12 @@
         <v>170</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>174</v>
@@ -4355,12 +4343,12 @@
         <v>170</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>177</v>
@@ -4381,12 +4369,12 @@
         <v>170</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>177</v>
@@ -4404,15 +4392,15 @@
         <v>172</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>177</v>
@@ -4433,12 +4421,12 @@
         <v>170</v>
       </c>
       <c r="H6" s="67" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>177</v>
@@ -4459,12 +4447,12 @@
         <v>170</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>177</v>
@@ -4485,10 +4473,10 @@
         <v>170</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="46" t="s">
         <v>182</v>
       </c>
@@ -4514,9 +4502,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>250</v>
+        <v>183</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>183</v>
@@ -4537,12 +4525,12 @@
         <v>170</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>251</v>
+        <v>186</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>186</v>
@@ -4563,12 +4551,12 @@
         <v>170</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>189</v>
@@ -4589,12 +4577,12 @@
         <v>170</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>189</v>
@@ -4612,15 +4600,15 @@
         <v>172</v>
       </c>
       <c r="G13" s="66" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>189</v>
@@ -4641,12 +4629,12 @@
         <v>170</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>189</v>
@@ -4667,12 +4655,12 @@
         <v>170</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>189</v>
@@ -4693,10 +4681,10 @@
         <v>170</v>
       </c>
       <c r="H16" s="67" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="46" t="s">
         <v>182</v>
       </c>
@@ -4722,9 +4710,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B18" s="59" t="s">
         <v>194</v>
@@ -4745,12 +4733,12 @@
         <v>170</v>
       </c>
       <c r="H18" s="67" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B19" s="59" t="s">
         <v>194</v>
@@ -4771,13 +4759,13 @@
         <v>170</v>
       </c>
       <c r="H19" s="67" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="J19" s="67"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="B20" s="59" t="s">
         <v>199</v>
@@ -4798,12 +4786,12 @@
         <v>170</v>
       </c>
       <c r="H20" s="67" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B21" s="59" t="s">
         <v>202</v>
@@ -4824,12 +4812,12 @@
         <v>170</v>
       </c>
       <c r="H21" s="67" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B22" s="59" t="s">
         <v>202</v>
@@ -4850,12 +4838,12 @@
         <v>170</v>
       </c>
       <c r="H22" s="67" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B23" s="59" t="s">
         <v>202</v>
@@ -4876,12 +4864,12 @@
         <v>170</v>
       </c>
       <c r="H23" s="67" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B24" s="59" t="s">
         <v>202</v>
@@ -4902,12 +4890,12 @@
         <v>170</v>
       </c>
       <c r="H24" s="67" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="65" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B25" s="59" t="s">
         <v>202</v>
@@ -4928,12 +4916,12 @@
         <v>170</v>
       </c>
       <c r="H25" s="60" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>268</v>
+        <v>205</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>205</v>
@@ -4954,7 +4942,7 @@
         <v>170</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4980,7 +4968,7 @@
         <v>170</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5006,7 +4994,7 @@
         <v>170</v>
       </c>
       <c r="H28" s="60" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5032,7 +5020,7 @@
         <v>170</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,12 +5046,12 @@
         <v>170</v>
       </c>
       <c r="H30" s="60" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>223</v>
@@ -5084,12 +5072,12 @@
         <v>170</v>
       </c>
       <c r="H31" s="60" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>223</v>
@@ -5110,12 +5098,12 @@
         <v>170</v>
       </c>
       <c r="H32" s="60" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>223</v>
@@ -5136,12 +5124,12 @@
         <v>170</v>
       </c>
       <c r="H33" s="60" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>223</v>
@@ -5162,15 +5150,15 @@
         <v>170</v>
       </c>
       <c r="H34" s="60" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="35" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C35" s="44" t="n">
         <v>8</v>
@@ -5188,15 +5176,15 @@
         <v>170</v>
       </c>
       <c r="H35" s="67" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="65" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="C36" s="44" t="n">
         <v>0</v>
@@ -5214,15 +5202,15 @@
         <v>170</v>
       </c>
       <c r="H36" s="67" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="35" t="s">
-        <v>286</v>
+        <v>228</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="C37" s="44" t="n">
         <v>0</v>
@@ -5240,15 +5228,15 @@
         <v>170</v>
       </c>
       <c r="H37" s="67" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="35" t="s">
-        <v>288</v>
+        <v>220</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="C38" s="44" t="n">
         <v>0</v>
@@ -5266,7 +5254,7 @@
         <v>170</v>
       </c>
       <c r="H38" s="62" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5309,13 +5297,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="C1" s="45" t="s">
         <v>233</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>234</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -5366,16 +5354,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>78</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E1" s="68" t="s">
         <v>11</v>
@@ -5383,7 +5371,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B2" s="44" t="n">
         <v>6</v>
@@ -5392,49 +5380,49 @@
         <v>170</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B3" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B4" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B5" s="44" t="n">
         <v>6</v>
@@ -5443,100 +5431,100 @@
         <v>178</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B6" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B7" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B8" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D8" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>306</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B9" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B10" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B11" s="44" t="n">
         <v>6</v>
@@ -5545,15 +5533,15 @@
         <v>190</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B12" s="44" t="n">
         <v>6</v>
@@ -5562,44 +5550,44 @@
         <v>200</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B13" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D13" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>321</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B14" s="44" t="n">
         <v>6</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5620,8 +5608,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5637,10 +5625,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>104</v>
@@ -5649,7 +5637,7 @@
         <v>78</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F1" s="68" t="s">
         <v>11</v>
@@ -5657,10 +5645,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C2" s="44" t="n">
         <v>8</v>
@@ -5674,10 +5662,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C3" s="44" t="n">
         <v>0</v>
@@ -5686,15 +5674,15 @@
         <v>3</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C4" s="44" t="n">
         <v>8</v>
@@ -5703,15 +5691,15 @@
         <v>6</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C5" s="44" t="n">
         <v>0</v>
@@ -5720,15 +5708,15 @@
         <v>3</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C6" s="44" t="n">
         <v>8</v>
@@ -5737,15 +5725,15 @@
         <v>6</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C7" s="44" t="n">
         <v>0</v>
@@ -5754,15 +5742,15 @@
         <v>3</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C8" s="44" t="n">
         <v>8</v>
@@ -5776,10 +5764,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C9" s="44" t="n">
         <v>0</v>
@@ -5788,15 +5776,15 @@
         <v>3</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C10" s="44" t="n">
         <v>8</v>
@@ -5805,15 +5793,15 @@
         <v>6</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C11" s="44" t="n">
         <v>0</v>
@@ -5822,15 +5810,15 @@
         <v>3</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C12" s="44" t="n">
         <v>8</v>
@@ -5839,15 +5827,15 @@
         <v>6</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C13" s="44" t="n">
         <v>0</v>
@@ -5856,15 +5844,15 @@
         <v>3</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C14" s="44" t="n">
         <v>8</v>
@@ -5873,15 +5861,15 @@
         <v>6</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C15" s="44" t="n">
         <v>0</v>
@@ -5890,15 +5878,15 @@
         <v>3</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C16" s="44" t="n">
         <v>8</v>
@@ -5907,15 +5895,15 @@
         <v>6</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C17" s="44" t="n">
         <v>0</v>
@@ -5924,15 +5912,15 @@
         <v>3</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C18" s="44" t="n">
         <v>8</v>
@@ -5941,15 +5929,15 @@
         <v>6</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C19" s="44" t="n">
         <v>0</v>
@@ -5958,15 +5946,15 @@
         <v>3</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C20" s="44" t="n">
         <v>8</v>
@@ -5975,15 +5963,15 @@
         <v>6</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>190</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C21" s="44" t="n">
         <v>0</v>
@@ -5992,15 +5980,15 @@
         <v>3</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C22" s="44" t="n">
         <v>8</v>
@@ -6009,15 +5997,15 @@
         <v>6</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C23" s="44" t="n">
         <v>0</v>
@@ -6026,15 +6014,15 @@
         <v>3</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C24" s="44" t="n">
         <v>8</v>
@@ -6043,15 +6031,15 @@
         <v>6</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C25" s="44" t="n">
         <v>0</v>
@@ -6060,15 +6048,15 @@
         <v>3</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C26" s="44" t="n">
         <v>8</v>
@@ -6077,15 +6065,15 @@
         <v>6</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>331</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="35" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C27" s="44" t="n">
         <v>0</v>
@@ -6094,7 +6082,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>